<commit_message>
Create RG Test Case
Completed the Add Contact Section
</commit_message>
<xml_diff>
--- a/Input_TestData/ExcelSheet_TestData_UI.xlsx
+++ b/Input_TestData/ExcelSheet_TestData_UI.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\All_In_One\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik.hussain\git\HDAP2_PEGAUI_Automation\Input_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD02B07-55E6-4295-9044-03BE19E0A0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FBEF72-0881-46BA-A9CC-779B8F5E6559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alphaSheet" sheetId="1" r:id="rId1"/>
     <sheet name="betaSheet" sheetId="2" r:id="rId2"/>
     <sheet name="realTime" sheetId="3" r:id="rId3"/>
+    <sheet name="createRG" sheetId="4" r:id="rId4"/>
+    <sheet name="preLaunch" sheetId="5" r:id="rId5"/>
+    <sheet name="DQA" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="122">
   <si>
     <t>attribute1</t>
   </si>
@@ -276,6 +279,123 @@
   </si>
   <si>
     <t>543543</t>
+  </si>
+  <si>
+    <t>happyPath</t>
+  </si>
+  <si>
+    <t>contactType</t>
+  </si>
+  <si>
+    <t>department</t>
+  </si>
+  <si>
+    <t>ext</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>fax</t>
+  </si>
+  <si>
+    <t>preferredMethod</t>
+  </si>
+  <si>
+    <t>sameAsRequestGroup</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Billing</t>
+  </si>
+  <si>
+    <t>Phi Automation Team</t>
+  </si>
+  <si>
+    <t>Testing Team</t>
+  </si>
+  <si>
+    <t>phiteam@test.com</t>
+  </si>
+  <si>
+    <t>US/Alaska</t>
+  </si>
+  <si>
+    <t>8,</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>"9642869555"</t>
+  </si>
+  <si>
+    <t>"8"</t>
+  </si>
+  <si>
+    <t>"8529637415"</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>requestGroupName</t>
+  </si>
+  <si>
+    <t>timeZoneRG</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>retrievalMethods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vinay Automation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated Instructions </t>
+  </si>
+  <si>
+    <t>wfSettingOwner</t>
+  </si>
+  <si>
+    <t>Zakirshaik</t>
+  </si>
+  <si>
+    <t>timeZoneContact</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>onlyOwnerWork</t>
+  </si>
+  <si>
+    <t>ContactWillLetter</t>
+  </si>
+  <si>
+    <t>ContactWillConfirm</t>
+  </si>
+  <si>
+    <t>ExcludeFromBulk</t>
+  </si>
+  <si>
+    <t>ReasonExclusion</t>
+  </si>
+  <si>
+    <t>WebSite</t>
   </si>
 </sst>
 </file>
@@ -318,7 +438,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -354,11 +474,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -370,6 +501,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,21 +802,21 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="8"/>
-    <col min="10" max="10" width="9.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.109375" style="8"/>
+    <col min="1" max="1" width="12.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.08984375" style="8"/>
+    <col min="10" max="10" width="9.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.08984375" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -696,7 +842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
         <v>54</v>
@@ -717,7 +863,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -737,7 +883,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>18</v>
@@ -752,7 +898,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
@@ -778,7 +924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>65</v>
@@ -799,7 +945,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
@@ -837,7 +983,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>79</v>
@@ -870,7 +1016,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>70</v>
       </c>
@@ -890,7 +1036,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
         <v>71</v>
@@ -920,19 +1066,19 @@
       <selection activeCell="A3" sqref="A3:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -958,7 +1104,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -979,7 +1125,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -999,7 +1145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -1014,7 +1160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1040,7 +1186,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -1061,7 +1207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -1099,7 +1245,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
@@ -1141,19 +1287,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0703D59-0802-4774-9111-52139DE76A14}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
@@ -1167,7 +1313,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="4" t="s">
         <v>75</v>
@@ -1180,4 +1326,206 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE91C4FB-E20E-468F-AACF-33BCD7A988CB}">
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.90625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.6328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.81640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="30" width="8.7265625" style="11"/>
+    <col min="31" max="31" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="8.7265625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="W1" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE1" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="T2" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{EB69ADFB-3F18-4E42-A89A-39D385ED211C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C717FB09-8AC9-4ACF-9A0D-A8BA9DFD45B9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB2257F-F658-4FDD-978C-30EFA3D235AE}">
+  <dimension ref="P12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="12" spans="16:16" x14ac:dyDescent="0.35">
+      <c r="P12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Completed the code for RG Setting section
</commit_message>
<xml_diff>
--- a/Input_TestData/ExcelSheet_TestData_UI.xlsx
+++ b/Input_TestData/ExcelSheet_TestData_UI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hi\git\HDAP2_PEGAUI_Automation\Input_TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaik.hussain\git\HDAP2_PEGAUI_Automation\Input_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED55251B-5BD9-4179-8B47-5A1076C27C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE219647-C37A-4D57-B20B-DC17600C981B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="190">
   <si>
     <t>attribute1</t>
   </si>
@@ -380,9 +380,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>onlyOwnerWork</t>
-  </si>
-  <si>
     <t>ContactWillLetter</t>
   </si>
   <si>
@@ -398,24 +395,6 @@
     <t>WebSite</t>
   </si>
   <si>
-    <t>MS_AttnTo</t>
-  </si>
-  <si>
-    <t>MS_Address</t>
-  </si>
-  <si>
-    <t>MS_Address_Line2</t>
-  </si>
-  <si>
-    <t>MS__City</t>
-  </si>
-  <si>
-    <t>MS_State</t>
-  </si>
-  <si>
-    <t>MS_Zip_Code</t>
-  </si>
-  <si>
     <t>LP_SendingLetterCheck_ddl</t>
   </si>
   <si>
@@ -476,21 +455,12 @@
     <t>PayVia_ddl</t>
   </si>
   <si>
-    <t>PayPreference_CheckDDL</t>
-  </si>
-  <si>
-    <t>PaymentPreference_None</t>
-  </si>
-  <si>
     <t>ReturnPreference_DDL</t>
   </si>
   <si>
     <t>SP_DDL</t>
   </si>
   <si>
-    <t>SP_Usemailaddress_Checkbox</t>
-  </si>
-  <si>
     <t>SP_AttnTo_textbox</t>
   </si>
   <si>
@@ -543,6 +513,93 @@
   </si>
   <si>
     <t>Need account number/other info added to request</t>
+  </si>
+  <si>
+    <t>MA_AttnTo</t>
+  </si>
+  <si>
+    <t>Kurnool</t>
+  </si>
+  <si>
+    <t>MA_Address</t>
+  </si>
+  <si>
+    <t>MA_Address_Line2</t>
+  </si>
+  <si>
+    <t>MA__City</t>
+  </si>
+  <si>
+    <t>MA_State</t>
+  </si>
+  <si>
+    <t>MA_Zip_Code</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>SP_Usemainaddress_Checkbox</t>
+  </si>
+  <si>
+    <t>PrakashNagar</t>
+  </si>
+  <si>
+    <t>Colony1</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>"55447"</t>
+  </si>
+  <si>
+    <t>Arif</t>
+  </si>
+  <si>
+    <t>Ghandi Nagar</t>
+  </si>
+  <si>
+    <t>Road No4</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>84043</t>
+  </si>
+  <si>
+    <t>"51524"</t>
+  </si>
+  <si>
+    <t>Santosh Nagar</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>OnlyOwnerWork</t>
+  </si>
+  <si>
+    <t>Naipet</t>
+  </si>
+  <si>
+    <t>Select Preference</t>
+  </si>
+  <si>
+    <t>Kothapeta</t>
   </si>
 </sst>
 </file>
@@ -642,7 +699,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -667,6 +724,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -955,21 +1018,21 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.08984375" style="8"/>
-    <col min="10" max="10" width="9.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.08984375" style="8"/>
+    <col min="1" max="1" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="8"/>
+    <col min="10" max="10" width="9.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -995,7 +1058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
         <v>54</v>
@@ -1016,7 +1079,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -1036,7 +1099,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>18</v>
@@ -1051,7 +1114,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
@@ -1077,7 +1140,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>65</v>
@@ -1098,7 +1161,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
@@ -1136,7 +1199,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>79</v>
@@ -1169,7 +1232,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>70</v>
       </c>
@@ -1189,7 +1252,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
         <v>71</v>
@@ -1219,19 +1282,19 @@
       <selection activeCell="A3" sqref="A3:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -1257,7 +1320,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -1278,7 +1341,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -1298,7 +1361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -1313,7 +1376,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1339,7 +1402,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -1360,7 +1423,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -1398,7 +1461,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
@@ -1444,15 +1507,15 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
@@ -1466,7 +1529,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="4" t="s">
         <v>75</v>
@@ -1485,84 +1548,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE91C4FB-E20E-468F-AACF-33BCD7A988CB}">
   <dimension ref="A1:BP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BF1" sqref="BF1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="44.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.7265625" style="11"/>
-    <col min="28" max="28" width="8.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="20.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="23.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="20.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="22.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="27.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="21.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="21.453125" style="11" customWidth="1"/>
-    <col min="48" max="48" width="12.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="22.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="23.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20.6328125" style="11" customWidth="1"/>
-    <col min="53" max="53" width="7.6328125" style="11" customWidth="1"/>
-    <col min="54" max="54" width="27.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="19" style="11" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="18.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="22.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="11.36328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="18.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.90625" style="11" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="26.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="27.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="31.6328125" style="11" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="23.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="24.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="26.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="32.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="69" max="16384" width="8.7265625" style="11"/>
+    <col min="5" max="5" width="11.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="44.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="26.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="20.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="21.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="11" customWidth="1"/>
+    <col min="48" max="48" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="20.5703125" style="11" customWidth="1"/>
+    <col min="51" max="51" width="7.5703125" style="11" customWidth="1"/>
+    <col min="52" max="52" width="27.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19" style="11" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16" style="11" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="27.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="27.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="31.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="23.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="24.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="26.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="32.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="67" max="68" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="69" max="16384" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:68" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>83</v>
       </c>
@@ -1614,161 +1675,161 @@
       <c r="Q1" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="S1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="T1" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="V1" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="W1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y1" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z1" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="AC1" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD1" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="AE1" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="Y1" s="14" t="s">
+      <c r="AF1" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="AG1" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="AA1" s="14" t="s">
+      <c r="AH1" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AI1" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="AC1" s="14" t="s">
+      <c r="AJ1" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="AD1" s="14" t="s">
+      <c r="AK1" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="AE1" s="15" t="s">
+      <c r="AL1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AM1" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="AG1" s="14" t="s">
+      <c r="AN1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO1" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="AH1" s="14" t="s">
+      <c r="AP1" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="AI1" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="AJ1" s="14" t="s">
+      <c r="AQ1" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="AK1" s="14" t="s">
+      <c r="AR1" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="AL1" s="14" t="s">
+      <c r="AS1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="AM1" s="14" t="s">
+      <c r="AT1" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="AN1" s="14" t="s">
+      <c r="AU1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AV1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="AW1" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="AO1" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP1" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="AQ1" s="14" t="s">
+      <c r="AX1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="AR1" s="15" t="s">
+      <c r="AY1" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AZ1" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="BA1" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="AT1" s="14" t="s">
+      <c r="BB1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="AU1" s="14" t="s">
+      <c r="BC1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="BD1" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="AV1" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="AW1" s="14" t="s">
+      <c r="BE1" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="AX1" s="14" t="s">
+      <c r="BF1" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="AY1" s="14" t="s">
+      <c r="BG1" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="AZ1" s="14" t="s">
+      <c r="BH1" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="BA1" s="14" t="s">
+      <c r="BI1" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="BB1" s="14" t="s">
+      <c r="BJ1" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="BC1" s="14" t="s">
+      <c r="BK1" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="BD1" s="14" t="s">
+      <c r="BL1" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="BE1" s="14" t="s">
+      <c r="BM1" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="BF1" s="14" t="s">
+      <c r="BN1" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="BG1" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="BH1" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="BI1" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="BJ1" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="BK1" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="BL1" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="BM1" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="BN1" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="BO1" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="BP1" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:68" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="BO1" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="BP1" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:68" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>92</v>
       </c>
@@ -1817,25 +1878,122 @@
       <c r="Q2" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="R2" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="V2" s="14" t="s">
+      <c r="R2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="X2" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="Y2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC2" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AD2" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="AV2" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="W2" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AW2" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="AX2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY2" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="AZ2" s="12"/>
+      <c r="BA2" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="BB2" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="BC2" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="BD2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="BE2" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="BF2" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="BG2" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="BH2" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="BI2" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="BJ2" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="BK2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="BL2" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="BM2" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="BN2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="BO2" s="14" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1854,7 +2012,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1868,9 +2026,9 @@
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="12" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
Create RG Test Cases
</commit_message>
<xml_diff>
--- a/Input_TestData/ExcelSheet_TestData_UI.xlsx
+++ b/Input_TestData/ExcelSheet_TestData_UI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hi\git\HDAP2_PEGAUI_Automation\Input_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4FFFA3-6F12-42A4-AF63-C58A3B22B476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4481C1-1DCA-434A-9BCD-7FDE50DD574B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alphaSheet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="193">
   <si>
     <t>attribute1</t>
   </si>
@@ -564,13 +564,58 @@
   </si>
   <si>
     <t>SPUsedRequestGroup_Checkbox</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>sendPrefereneceEmail</t>
+  </si>
+  <si>
+    <t>SP_Email</t>
+  </si>
+  <si>
+    <t>sendphiteam@testing.com</t>
+  </si>
+  <si>
+    <t>sendPreferenceEmail</t>
+  </si>
+  <si>
+    <t>sendPrefereneceFax</t>
+  </si>
+  <si>
+    <t>sendPreferenceFax</t>
+  </si>
+  <si>
+    <t>SP_Fax_Number</t>
+  </si>
+  <si>
+    <t>"998877665"</t>
+  </si>
+  <si>
+    <t>sendPrefereneceUpload</t>
+  </si>
+  <si>
+    <t>sendPreferenceUpload</t>
+  </si>
+  <si>
+    <t>Upload</t>
+  </si>
+  <si>
+    <t>SP_Upload_URL</t>
+  </si>
+  <si>
+    <t>sendPrefereneceMain_Checkbox</t>
+  </si>
+  <si>
+    <t>SP_UseMain_Checkbox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -587,6 +632,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -660,10 +713,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -693,8 +747,12 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -979,21 +1037,21 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="8"/>
-    <col min="10" max="10" width="9.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="8"/>
+    <col min="1" max="1" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="8"/>
+    <col min="10" max="10" width="9.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +1077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
         <v>54</v>
@@ -1040,7 +1098,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
@@ -1060,7 +1118,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
         <v>18</v>
@@ -1075,7 +1133,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
@@ -1101,7 +1159,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>65</v>
@@ -1122,7 +1180,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
@@ -1160,7 +1218,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>79</v>
@@ -1193,7 +1251,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>70</v>
       </c>
@@ -1213,7 +1271,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
         <v>71</v>
@@ -1243,19 +1301,19 @@
       <selection activeCell="A3" sqref="A3:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -1281,7 +1339,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -1302,7 +1360,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -1322,7 +1380,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>18</v>
@@ -1337,7 +1395,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1363,7 +1421,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -1384,7 +1442,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>45</v>
       </c>
@@ -1422,7 +1480,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>21</v>
@@ -1468,15 +1526,15 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>72</v>
       </c>
@@ -1490,7 +1548,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="4" t="s">
         <v>75</v>
@@ -1507,84 +1565,83 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE91C4FB-E20E-468F-AACF-33BCD7A988CB}">
-  <dimension ref="A1:BI2"/>
+  <dimension ref="A1:BI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AT3" sqref="AT3"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BA16" sqref="BA16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="44.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="20.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="21.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="22.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="21.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="23.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="20.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="22.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="27.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="21.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="23.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="21.453125" style="11" customWidth="1"/>
-    <col min="48" max="48" width="12.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="20.54296875" style="11" customWidth="1"/>
-    <col min="51" max="51" width="7.54296875" style="11" customWidth="1"/>
-    <col min="52" max="52" width="27.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="19" style="11" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="19.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="22.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="14.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="12.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="19.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="11" customWidth="1"/>
+    <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="52" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="20.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="23.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="21.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="11" customWidth="1"/>
+    <col min="48" max="48" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="20.5703125" style="11" customWidth="1"/>
+    <col min="51" max="51" width="8.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="27.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="33.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="19.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="22.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="12.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="19.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="16" style="11" customWidth="1"/>
-    <col min="60" max="60" width="27.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="27.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="31.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="23.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="24.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="26.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="32.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="10.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="68" max="16384" width="8.7265625" style="11"/>
+    <col min="60" max="60" width="27.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="27.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="31.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="23.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="24.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="26.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="32.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="68" max="16384" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:61" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>83</v>
       </c>
@@ -1769,7 +1826,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:61" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:61" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>92</v>
       </c>
@@ -1896,7 +1953,9 @@
       <c r="AY2" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="AZ2" s="12"/>
+      <c r="AZ2" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="BA2" s="12" t="s">
         <v>173</v>
       </c>
@@ -1921,11 +1980,1195 @@
       <c r="BH2" s="14" t="s">
         <v>149</v>
       </c>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="S3" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z3" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA3" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB3" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC3" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD3" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE3" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF3" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH3" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI3" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AJ3" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK3" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL3" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM3" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN3" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO3" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP3" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ3" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AR3" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS3" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="AT3" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU3" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV3" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW3" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX3" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY3" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ3" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="BA3" s="13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC4" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="12"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AS4" s="12"/>
+      <c r="AT4" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU4" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV4" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="AW4" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="AX4" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY4" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="AZ4" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="BA4" s="12"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="R5" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="T5" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="W5" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="X5" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y5" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z5" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA5" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB5" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC5" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD5" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE5" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF5" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH5" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI5" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AJ5" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK5" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL5" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM5" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN5" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP5" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ5" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AR5" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS5" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="AT5" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU5" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV5" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW5" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX5" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY5" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ5" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="BA5" s="13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
+      <c r="B6" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="R6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="U6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="W6" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="X6" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y6" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z6" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA6" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB6" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC6" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ6" s="12"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="12"/>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="12"/>
+      <c r="AO6" s="12"/>
+      <c r="AP6" s="12"/>
+      <c r="AQ6" s="12"/>
+      <c r="AR6" s="12"/>
+      <c r="AS6" s="12"/>
+      <c r="AT6" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU6" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV6" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="AW6" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="AX6" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="AZ6" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="BA6" s="12"/>
+    </row>
+    <row r="7" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="X7" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y7" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA7" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB7" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC7" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD7" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE7" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF7" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG7" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH7" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI7" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AJ7" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK7" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL7" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM7" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN7" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO7" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP7" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ7" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AR7" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS7" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="AT7" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU7" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV7" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW7" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX7" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY7" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ7" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="BA7" s="13" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q8" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="R8" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="U8" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="V8" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="W8" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="X8" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y8" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z8" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA8" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB8" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC8" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD8" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE8" s="12"/>
+      <c r="AF8" s="12"/>
+      <c r="AG8" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH8" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI8" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ8" s="12"/>
+      <c r="AK8" s="12"/>
+      <c r="AL8" s="12"/>
+      <c r="AM8" s="12"/>
+      <c r="AN8" s="12"/>
+      <c r="AO8" s="12"/>
+      <c r="AP8" s="12"/>
+      <c r="AQ8" s="12"/>
+      <c r="AR8" s="12"/>
+      <c r="AS8" s="12"/>
+      <c r="AT8" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU8" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV8" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="AW8" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="AX8" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY8" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="AZ8" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="BA8" s="12"/>
+    </row>
+    <row r="9" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q9" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="R9" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="U9" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="V9" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="W9" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="X9" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y9" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z9" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA9" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB9" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="AC9" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD9" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE9" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF9" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG9" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="AH9" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI9" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="AJ9" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK9" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL9" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM9" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN9" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO9" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP9" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ9" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AR9" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS9" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="AT9" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU9" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV9" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="AW9" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX9" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY9" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ9" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="BA9" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="S10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="U10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="V10" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="W10" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="X10" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y10" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z10" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA10" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB10" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC10" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="AD10" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AJ10" s="12"/>
+      <c r="AK10" s="12"/>
+      <c r="AL10" s="12"/>
+      <c r="AM10" s="12"/>
+      <c r="AN10" s="12"/>
+      <c r="AO10" s="12"/>
+      <c r="AP10" s="12"/>
+      <c r="AQ10" s="12"/>
+      <c r="AR10" s="12"/>
+      <c r="AS10" s="12"/>
+      <c r="AT10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU10" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV10" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="AW10" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="AX10" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="AY10" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="AZ10" s="17"/>
+      <c r="BA10" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{EB69ADFB-3F18-4E42-A89A-39D385ED211C}"/>
     <hyperlink ref="W2" r:id="rId2" xr:uid="{4B6AA15B-5658-44FA-86E3-E2F03BEA3927}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{3F0AD587-D7D7-4830-B390-5685B6650D54}"/>
+    <hyperlink ref="W4" r:id="rId4" xr:uid="{1CB29270-D53E-497B-B221-1C4752E4D5F1}"/>
+    <hyperlink ref="AZ4" r:id="rId5" xr:uid="{49C31D5B-3604-4777-9AC1-3A57F81F9B1B}"/>
+    <hyperlink ref="F6" r:id="rId6" xr:uid="{7E1F67B4-38D7-430E-820D-6C95C7241C35}"/>
+    <hyperlink ref="W6" r:id="rId7" xr:uid="{62E52780-99F0-4E22-82BD-BAA2EBDE85F5}"/>
+    <hyperlink ref="F8" r:id="rId8" xr:uid="{B7E2EEE4-8167-4A78-9AEF-F7042E840E59}"/>
+    <hyperlink ref="W8" r:id="rId9" xr:uid="{0491D8A9-8068-4094-96E5-2BDEFBFB27F6}"/>
+    <hyperlink ref="AZ8" r:id="rId10" xr:uid="{CA9E29FD-BE25-4853-BFF8-E65797357153}"/>
+    <hyperlink ref="F10" r:id="rId11" xr:uid="{208FC354-E239-4A69-871F-467B89CBF3C0}"/>
+    <hyperlink ref="W10" r:id="rId12" xr:uid="{A080488D-EC64-40A3-B397-859ADEDBC102}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1937,7 +3180,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1951,9 +3194,9 @@
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="12" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
         <v>98</v>
       </c>

</xml_diff>